<commit_message>
Compilation is progressing albeit slowly...
</commit_message>
<xml_diff>
--- a/Whitepaper/competitors.xlsx
+++ b/Whitepaper/competitors.xlsx
@@ -1,21 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Marci\Suli\Year 3\CS3028\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/albert-private/Desktop/Desktop/Uni/Year 3/Winter Semester/Software Engineering/Portfolio-backtesting/Whitepaper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABF3B0AC-5CB2-416A-9809-326383734EFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5AAFF45-FE57-F445-B111-46EFD34055FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="3480" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{95FB7CF1-23F3-4E32-B2A6-5F9F1DA043D7}"/>
+    <workbookView xWindow="-38400" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{95FB7CF1-23F3-4E32-B2A6-5F9F1DA043D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
     <sheet name="Munka2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Munka1!$B$13:$B$16</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Munka1!$E$13:$E$16</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">Munka1!$B$13:$B$16</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">Munka1!$E$13:$E$16</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">Munka1!$E$2:$E$12</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">Munka1!$B$13:$B$16</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">Munka1!$E$13:$E$16</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">Munka1!$E$2:$E$12</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">Munka1!$B$13:$B$16</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">Munka1!$E$13:$E$16</definedName>
+    <definedName name="_xlchart.v1.18" hidden="1">Munka1!$E$2:$E$12</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Munka1!$E$2:$E$12</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Munka1!$B$13:$B$16</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Munka1!$E$13:$E$16</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Munka1!$E$2:$E$12</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Munka1!$B$2:$B$12</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Munka1!$E$2:$E$12</definedName>
+    <definedName name="_xlchart.v2.6" hidden="1">Munka1!$B$2:$B$12</definedName>
+    <definedName name="_xlchart.v2.7" hidden="1">Munka1!$E$2:$E$12</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -32,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
   <si>
     <t>MultiCharts</t>
   </si>
@@ -80,9 +101,6 @@
   </si>
   <si>
     <t>Equities Lab</t>
-  </si>
-  <si>
-    <t>Institutional grade</t>
   </si>
   <si>
     <t>Strategy Quant</t>
@@ -152,7 +170,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normál" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -170,7 +188,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="hu-HU"/>
+  <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -202,7 +220,15 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="hu-HU"/>
-              <a:t>Price of a prinancial software per month</a:t>
+              <a:t>MONTHLY</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="hu-HU" baseline="0"/>
+              <a:t> PRICE OF EXISTING BACKTESTING </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="hu-HU"/>
+              <a:t>software</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -247,7 +273,7 @@
           <c:idx val="1"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Incldues trading</c:v>
+            <c:v>Includes Trading</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -287,7 +313,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="50000"/>
@@ -302,13 +328,14 @@
                 <a:endParaRPr lang="de-DE"/>
               </a:p>
             </c:txPr>
-            <c:dLblPos val="t"/>
+            <c:dLblPos val="b"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="1"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
+            <c:separator> </c:separator>
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
@@ -329,108 +356,11 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
-          <c:errBars>
-            <c:errDir val="y"/>
-            <c:errBarType val="both"/>
-            <c:errValType val="cust"/>
-            <c:noEndCap val="0"/>
-            <c:plus>
-              <c:numRef>
-                <c:f>Munka1!$G$2:$G$11</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="10"/>
-                  <c:pt idx="0">
-                    <c:v>16.291666666666657</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>25</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>2.5416666666666679</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>150</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>15.049999999999997</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>22.916666666666668</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>75</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>125</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:plus>
-            <c:minus>
-              <c:numRef>
-                <c:f>Munka1!$C$2:$C$11</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="10"/>
-                  <c:pt idx="0">
-                    <c:v>16.291666666666671</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>25</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>2.5416666666666643</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>150</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>15.050000000000004</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>22.916666666666664</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>75</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>125</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:minus>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
           <c:xVal>
             <c:strRef>
-              <c:f>Munka1!$B$2:$B$13</c:f>
+              <c:f>Munka1!$B$2:$B$12</c:f>
               <c:strCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>MultiCharts</c:v>
                 </c:pt>
@@ -462,9 +392,6 @@
                   <c:v>eSignal</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>Institutional grade</c:v>
-                </c:pt>
-                <c:pt idx="11">
                   <c:v>Strategy Quant</c:v>
                 </c:pt>
               </c:strCache>
@@ -472,10 +399,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Munka1!$E$2:$E$13</c:f>
+              <c:f>Munka1!$E$2:$E$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>82.708333333333343</c:v>
                 </c:pt>
@@ -507,9 +434,6 @@
                   <c:v>170</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>199</c:v>
-                </c:pt>
-                <c:pt idx="11">
                   <c:v>124.16666666666667</c:v>
                 </c:pt>
               </c:numCache>
@@ -526,7 +450,7 @@
           <c:idx val="0"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Trading not included</c:v>
+            <c:v>Trading Excluded</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -560,13 +484,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="36576" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
                 <a:spAutoFit/>
               </a:bodyPr>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="50000"/>
@@ -584,13 +508,23 @@
             <c:dLblPos val="t"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
-            <c:showCatName val="0"/>
+            <c:showCatName val="1"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
+            <c:separator> </c:separator>
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <a:prstGeom prst="rect">
+                    <a:avLst/>
+                  </a:prstGeom>
+                  <a:noFill/>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                </c15:spPr>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -609,29 +543,28 @@
             </c:extLst>
           </c:dLbls>
           <c:xVal>
-            <c:numRef>
-              <c:f>Munka1!$A$14:$A$17</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
+            <c:strRef>
+              <c:f>Munka1!$B$13:$B$16</c:f>
+              <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>13</c:v>
+                  <c:v>Portfolio123</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14</c:v>
+                  <c:v>Equities Lab</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15</c:v>
+                  <c:v>ETFreplay</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16</c:v>
+                  <c:v>Genovest</c:v>
                 </c:pt>
-              </c:numCache>
-            </c:numRef>
+              </c:strCache>
+            </c:strRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Munka1!$E$14:$E$17</c:f>
+              <c:f>Munka1!$E$13:$E$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
@@ -693,7 +626,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
+        <c:tickLblPos val="none"/>
         <c:spPr>
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -736,7 +669,7 @@
         <c:axId val="368571136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="400"/>
+          <c:max val="300"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -754,6 +687,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE" sz="1200" baseline="0"/>
+                  <a:t>Price in $US</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -818,7 +806,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -1442,16 +1430,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>223837</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>147637</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1480,7 +1468,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-téma">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1776,45 +1764,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3961E5CC-0DA3-4F5C-9C48-97558AB33285}">
-  <dimension ref="A1:I74"/>
+  <dimension ref="A1:I73"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" customWidth="1"/>
-    <col min="4" max="8" width="11.28515625" customWidth="1"/>
+    <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5" customWidth="1"/>
+    <col min="4" max="8" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1843,10 +1831,10 @@
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1854,29 +1842,29 @@
         <v>4</v>
       </c>
       <c r="C3" s="2">
-        <f t="shared" ref="C3:C17" si="0">E3-D3</f>
+        <f t="shared" ref="C3:C16" si="0">E3-D3</f>
         <v>25</v>
       </c>
       <c r="D3" s="2">
         <v>250</v>
       </c>
       <c r="E3" s="2">
-        <f t="shared" ref="E3:E17" si="1">(D3+F3)/2</f>
+        <f t="shared" ref="E3:E16" si="1">(D3+F3)/2</f>
         <v>275</v>
       </c>
       <c r="F3" s="2">
         <v>300</v>
       </c>
       <c r="G3" s="2">
-        <f t="shared" ref="G3:G17" si="2">F3-E3</f>
+        <f t="shared" ref="G3:G16" si="2">F3-E3</f>
         <v>25</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1905,10 +1893,10 @@
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1935,10 +1923,10 @@
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1967,10 +1955,10 @@
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1997,10 +1985,10 @@
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -2028,10 +2016,10 @@
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -2059,10 +2047,10 @@
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -2089,10 +2077,10 @@
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -2119,192 +2107,173 @@
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C12" s="2">
-        <f t="shared" ref="C12:C13" si="3">E12-D12</f>
-        <v>100</v>
+        <f t="shared" ref="C12" si="3">E12-D12</f>
+        <v>0</v>
       </c>
       <c r="D12" s="2">
-        <v>99</v>
+        <f>1490/12</f>
+        <v>124.16666666666667</v>
       </c>
       <c r="E12" s="2">
         <f t="shared" si="1"/>
-        <v>199</v>
+        <v>124.16666666666667</v>
       </c>
       <c r="F12" s="2">
-        <v>299</v>
+        <f>1490/12</f>
+        <v>124.16666666666667</v>
       </c>
       <c r="G12" s="2">
-        <f t="shared" ref="G12:G13" si="4">F12-E12</f>
-        <v>100</v>
+        <f t="shared" ref="G12" si="4">F12-E12</f>
+        <v>0</v>
       </c>
       <c r="H12" s="2"/>
       <c r="I12" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C13" s="2">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>30</v>
       </c>
       <c r="D13" s="2">
-        <f>1490/12</f>
-        <v>124.16666666666667</v>
+        <v>139</v>
       </c>
       <c r="E13" s="2">
         <f t="shared" si="1"/>
-        <v>124.16666666666667</v>
+        <v>169</v>
       </c>
       <c r="F13" s="2">
-        <f>1490/12</f>
-        <v>124.16666666666667</v>
+        <v>199</v>
       </c>
       <c r="G13" s="2">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>30</v>
       </c>
       <c r="H13" s="2"/>
       <c r="I13" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C14" s="2">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>32.5</v>
       </c>
       <c r="D14" s="2">
-        <v>139</v>
+        <v>35</v>
       </c>
       <c r="E14" s="2">
         <f t="shared" si="1"/>
-        <v>169</v>
+        <v>67.5</v>
       </c>
       <c r="F14" s="2">
-        <v>199</v>
+        <v>100</v>
       </c>
       <c r="G14" s="2">
         <f t="shared" si="2"/>
-        <v>30</v>
+        <v>32.5</v>
       </c>
       <c r="H14" s="2"/>
       <c r="I14" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C15" s="2">
         <f t="shared" si="0"/>
-        <v>32.5</v>
+        <v>0</v>
       </c>
       <c r="D15" s="2">
-        <v>35</v>
+        <v>34.99</v>
       </c>
       <c r="E15" s="2">
         <f t="shared" si="1"/>
-        <v>67.5</v>
+        <v>34.99</v>
       </c>
       <c r="F15" s="2">
-        <v>100</v>
+        <v>34.99</v>
       </c>
       <c r="G15" s="2">
         <f t="shared" si="2"/>
-        <v>32.5</v>
+        <v>0</v>
       </c>
       <c r="H15" s="2"/>
       <c r="I15" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C16" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>12.5</v>
       </c>
       <c r="D16" s="2">
-        <v>34.99</v>
+        <v>25</v>
       </c>
       <c r="E16" s="2">
         <f t="shared" si="1"/>
-        <v>34.99</v>
+        <v>37.5</v>
       </c>
       <c r="F16" s="2">
-        <v>34.99</v>
+        <v>50</v>
       </c>
       <c r="G16" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>12.5</v>
       </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>16</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="2">
-        <f t="shared" si="0"/>
-        <v>12.5</v>
-      </c>
-      <c r="D17" s="2">
-        <v>25</v>
-      </c>
-      <c r="E17" s="2">
-        <f t="shared" si="1"/>
-        <v>37.5</v>
-      </c>
-      <c r="F17" s="2">
-        <v>50</v>
-      </c>
-      <c r="G17" s="2">
-        <f t="shared" si="2"/>
-        <v>12.5</v>
-      </c>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -2315,7 +2284,7 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -2326,7 +2295,7 @@
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -2337,7 +2306,7 @@
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -2348,7 +2317,7 @@
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -2359,7 +2328,7 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -2370,7 +2339,7 @@
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -2381,7 +2350,7 @@
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -2392,7 +2361,7 @@
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -2403,7 +2372,7 @@
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -2414,7 +2383,7 @@
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -2425,7 +2394,7 @@
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -2436,7 +2405,7 @@
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -2447,7 +2416,7 @@
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -2458,7 +2427,7 @@
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -2469,7 +2438,7 @@
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -2480,7 +2449,7 @@
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -2491,7 +2460,7 @@
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -2502,7 +2471,7 @@
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -2513,7 +2482,7 @@
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -2524,7 +2493,7 @@
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -2535,7 +2504,7 @@
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -2546,7 +2515,7 @@
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -2557,7 +2526,7 @@
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -2568,7 +2537,7 @@
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -2579,7 +2548,7 @@
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -2590,7 +2559,7 @@
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -2601,7 +2570,7 @@
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -2612,7 +2581,7 @@
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -2623,7 +2592,7 @@
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -2634,7 +2603,7 @@
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -2645,7 +2614,7 @@
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -2656,7 +2625,7 @@
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -2667,7 +2636,7 @@
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -2678,7 +2647,7 @@
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -2689,7 +2658,7 @@
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -2700,7 +2669,7 @@
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -2711,7 +2680,7 @@
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -2722,7 +2691,7 @@
       <c r="H55" s="1"/>
       <c r="I55" s="1"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -2733,7 +2702,7 @@
       <c r="H56" s="1"/>
       <c r="I56" s="1"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -2744,7 +2713,7 @@
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -2755,7 +2724,7 @@
       <c r="H58" s="1"/>
       <c r="I58" s="1"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -2766,7 +2735,7 @@
       <c r="H59" s="1"/>
       <c r="I59" s="1"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -2777,7 +2746,7 @@
       <c r="H60" s="1"/>
       <c r="I60" s="1"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -2788,7 +2757,7 @@
       <c r="H61" s="1"/>
       <c r="I61" s="1"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -2799,7 +2768,7 @@
       <c r="H62" s="1"/>
       <c r="I62" s="1"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -2810,7 +2779,7 @@
       <c r="H63" s="1"/>
       <c r="I63" s="1"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -2821,7 +2790,7 @@
       <c r="H64" s="1"/>
       <c r="I64" s="1"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -2832,7 +2801,7 @@
       <c r="H65" s="1"/>
       <c r="I65" s="1"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -2843,7 +2812,7 @@
       <c r="H66" s="1"/>
       <c r="I66" s="1"/>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -2854,7 +2823,7 @@
       <c r="H67" s="1"/>
       <c r="I67" s="1"/>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -2865,7 +2834,7 @@
       <c r="H68" s="1"/>
       <c r="I68" s="1"/>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -2876,7 +2845,7 @@
       <c r="H69" s="1"/>
       <c r="I69" s="1"/>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -2887,7 +2856,7 @@
       <c r="H70" s="1"/>
       <c r="I70" s="1"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -2898,7 +2867,7 @@
       <c r="H71" s="1"/>
       <c r="I71" s="1"/>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -2909,7 +2878,7 @@
       <c r="H72" s="1"/>
       <c r="I72" s="1"/>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -2919,17 +2888,6 @@
       <c r="G73" s="1"/>
       <c r="H73" s="1"/>
       <c r="I73" s="1"/>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A74" s="1"/>
-      <c r="B74" s="1"/>
-      <c r="C74" s="1"/>
-      <c r="D74" s="1"/>
-      <c r="E74" s="1"/>
-      <c r="F74" s="1"/>
-      <c r="G74" s="1"/>
-      <c r="H74" s="1"/>
-      <c r="I74" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2942,18 +2900,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{216B0A44-40EF-4167-B4A8-D25C868C402D}">
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="49" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="3"/>
+    <col min="2" max="2" width="15.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.1640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="3">
         <v>100</v>
       </c>
@@ -2970,7 +2928,7 @@
         <v>99.9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <f>A1*2</f>
         <v>200</v>
@@ -2992,9 +2950,9 @@
         <v>274.72500000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
-        <f t="shared" ref="A3:A36" si="2">A2*2</f>
+        <f t="shared" ref="A3:A10" si="2">A2*2</f>
         <v>400</v>
       </c>
       <c r="B3" s="3">
@@ -3014,7 +2972,7 @@
         <v>574.42500000000007</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <f t="shared" si="2"/>
         <v>800</v>
@@ -3036,7 +2994,7 @@
         <v>1173.825</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <f t="shared" si="2"/>
         <v>1600</v>
@@ -3058,7 +3016,7 @@
         <v>2372.625</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <f t="shared" si="2"/>
         <v>3200</v>
@@ -3080,7 +3038,7 @@
         <v>4770.2250000000004</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <f t="shared" si="2"/>
         <v>6400</v>
@@ -3102,7 +3060,7 @@
         <v>9565.4250000000011</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <f t="shared" si="2"/>
         <v>12800</v>
@@ -3124,7 +3082,7 @@
         <v>19155.825000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <f t="shared" si="2"/>
         <v>25600</v>
@@ -3146,7 +3104,7 @@
         <v>38336.625</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <f t="shared" si="2"/>
         <v>51200</v>
@@ -3168,7 +3126,7 @@
         <v>76698.225000000006</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <f>A10</f>
         <v>51200</v>
@@ -3190,7 +3148,7 @@
         <v>89485.425000000003</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <f t="shared" ref="A12:A36" si="4">A11</f>
         <v>51200</v>
@@ -3212,7 +3170,7 @@
         <v>102272.625</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <f t="shared" si="4"/>
         <v>51200</v>
@@ -3234,7 +3192,7 @@
         <v>115059.825</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <f t="shared" si="4"/>
         <v>51200</v>
@@ -3256,7 +3214,7 @@
         <v>127847.02500000001</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <f t="shared" si="4"/>
         <v>51200</v>
@@ -3278,7 +3236,7 @@
         <v>140634.22500000001</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <f t="shared" si="4"/>
         <v>51200</v>
@@ -3300,7 +3258,7 @@
         <v>153421.42500000002</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <f t="shared" si="4"/>
         <v>51200</v>
@@ -3322,7 +3280,7 @@
         <v>166208.625</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <f t="shared" si="4"/>
         <v>51200</v>
@@ -3344,7 +3302,7 @@
         <v>178995.82500000001</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <f t="shared" si="4"/>
         <v>51200</v>
@@ -3366,7 +3324,7 @@
         <v>191783.02499999999</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <f t="shared" si="4"/>
         <v>51200</v>
@@ -3388,7 +3346,7 @@
         <v>204570.22500000001</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <f t="shared" si="4"/>
         <v>51200</v>
@@ -3410,7 +3368,7 @@
         <v>217357.42500000002</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <f t="shared" si="4"/>
         <v>51200</v>
@@ -3432,7 +3390,7 @@
         <v>230144.625</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <f t="shared" si="4"/>
         <v>51200</v>
@@ -3454,7 +3412,7 @@
         <v>242931.82500000001</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <f t="shared" si="4"/>
         <v>51200</v>
@@ -3476,7 +3434,7 @@
         <v>255719.02499999999</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <f t="shared" si="4"/>
         <v>51200</v>
@@ -3498,7 +3456,7 @@
         <v>268506.22499999998</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <f t="shared" si="4"/>
         <v>51200</v>
@@ -3520,7 +3478,7 @@
         <v>281293.42499999999</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <f t="shared" si="4"/>
         <v>51200</v>
@@ -3542,7 +3500,7 @@
         <v>294080.625</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <f t="shared" si="4"/>
         <v>51200</v>
@@ -3564,7 +3522,7 @@
         <v>306867.82500000001</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <f t="shared" si="4"/>
         <v>51200</v>
@@ -3586,7 +3544,7 @@
         <v>319655.02500000002</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <f t="shared" si="4"/>
         <v>51200</v>
@@ -3608,7 +3566,7 @@
         <v>332442.22500000003</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <f t="shared" si="4"/>
         <v>51200</v>
@@ -3630,7 +3588,7 @@
         <v>345229.42499999999</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <f t="shared" si="4"/>
         <v>51200</v>
@@ -3652,7 +3610,7 @@
         <v>358016.625</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <f t="shared" si="4"/>
         <v>51200</v>
@@ -3674,7 +3632,7 @@
         <v>370803.82500000001</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <f t="shared" si="4"/>
         <v>51200</v>
@@ -3696,7 +3654,7 @@
         <v>383591.02500000002</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <f t="shared" si="4"/>
         <v>51200</v>
@@ -3718,7 +3676,7 @@
         <v>396378.22500000003</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
         <f t="shared" si="4"/>
         <v>51200</v>

</xml_diff>